<commit_message>
Calcular la ecuacion de la recta y generar valores aleatorios
</commit_message>
<xml_diff>
--- a/data/HOJA BASE PARA CALCULO1.xlsx
+++ b/data/HOJA BASE PARA CALCULO1.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joziv\Documents\AAA_projects\Calculo de inversion\Calculo-de-la-Rentabilidad\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2C35413-26F7-44C5-AE29-C9F7FD3C72BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="20115" windowHeight="8760" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="caso abc imptos 10%" sheetId="8" r:id="rId1"/>
@@ -12,7 +18,20 @@
     <sheet name="CASO ABC IMPTOS 30%" sheetId="5" r:id="rId3"/>
     <sheet name="Hoja blanco" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -106,11 +125,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -607,7 +626,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -617,11 +636,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify"/>
-    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -645,30 +660,30 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="9" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="9" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="9" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="9" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="9" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="9" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="9" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="9" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="9" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="9" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="9" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="9" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="9" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="9" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="9" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="9" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="8" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="8" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="8" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="9" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="9" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="9" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="9" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="9" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="9" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -706,21 +721,21 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="10" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="10" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="10" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -771,13 +786,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -815,7 +838,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -849,6 +872,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -883,9 +907,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1058,675 +1083,675 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N29"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.42578125" customWidth="1"/>
-    <col min="2" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" customWidth="1"/>
+    <col min="1" max="1" width="29.44140625" customWidth="1"/>
+    <col min="2" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="20.25">
-      <c r="A1" s="78" t="s">
+    <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="80"/>
-      <c r="I1" s="80"/>
-      <c r="J1" s="80"/>
-      <c r="K1" s="80"/>
-      <c r="L1" s="80"/>
-      <c r="M1" s="80"/>
-      <c r="N1" s="80"/>
-    </row>
-    <row r="2" spans="1:14" ht="13.5" thickBot="1"/>
-    <row r="3" spans="1:14" s="4" customFormat="1" ht="36.75" thickBot="1">
-      <c r="A3" s="12" t="s">
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="78"/>
+      <c r="K1" s="78"/>
+      <c r="L1" s="78"/>
+      <c r="M1" s="78"/>
+      <c r="N1" s="78"/>
+    </row>
+    <row r="2" spans="1:14" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:14" s="4" customFormat="1" ht="35.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="13">
+      <c r="B3" s="11">
         <v>1</v>
       </c>
-      <c r="C3" s="14">
+      <c r="C3" s="12">
         <f t="shared" ref="C3:N3" si="0">B3+1</f>
         <v>2</v>
       </c>
-      <c r="D3" s="14">
+      <c r="D3" s="12">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E3" s="14">
+      <c r="E3" s="12">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="F3" s="14">
+      <c r="F3" s="12">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G3" s="14">
+      <c r="G3" s="12">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="H3" s="14">
+      <c r="H3" s="12">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="I3" s="14">
+      <c r="I3" s="12">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="J3" s="14">
+      <c r="J3" s="12">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="K3" s="14">
+      <c r="K3" s="12">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="L3" s="14">
+      <c r="L3" s="12">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="M3" s="14">
+      <c r="M3" s="12">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="N3" s="15">
+      <c r="N3" s="13">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="18">
-      <c r="A4" s="16" t="s">
+    <row r="4" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A4" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="17">
+      <c r="B4" s="15">
         <f>-0.2*$B$20</f>
         <v>-28000</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="16">
         <f>-0.5*$B$20</f>
         <v>-70000</v>
       </c>
-      <c r="D4" s="18">
+      <c r="D4" s="16">
         <f>-0.3*$B$20</f>
         <v>-42000</v>
       </c>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18"/>
-      <c r="M4" s="18"/>
-      <c r="N4" s="19"/>
-    </row>
-    <row r="5" spans="1:14" ht="18">
-      <c r="A5" s="20" t="s">
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="17"/>
+    </row>
+    <row r="5" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A5" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22">
+      <c r="B5" s="19"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20">
         <f>-E7*(3/12)</f>
         <v>-4669.72</v>
       </c>
-      <c r="F5" s="22">
+      <c r="F5" s="20">
         <f>-F7*(3/12)+E7*(3/12)</f>
         <v>-931.94399999999951</v>
       </c>
-      <c r="G5" s="22">
+      <c r="G5" s="20">
         <f>-G7*(3/12)+F7*(3/12)</f>
         <v>-621.29600000000028</v>
       </c>
-      <c r="H5" s="22">
+      <c r="H5" s="20">
         <f t="shared" ref="H5:M5" si="1">-H7*(3/12)+G7*(3/12)</f>
         <v>-1244.5919999999996</v>
       </c>
-      <c r="I5" s="22">
+      <c r="I5" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J5" s="22">
+      <c r="J5" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K5" s="22">
+      <c r="K5" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L5" s="22">
+      <c r="L5" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M5" s="22">
+      <c r="M5" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N5" s="23">
+      <c r="N5" s="21">
         <f>SUM(E5:M5)*-1</f>
         <v>7467.5519999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="18">
-      <c r="A6" s="20" t="s">
+    <row r="6" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A6" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22">
+      <c r="B6" s="19"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20">
         <f>0.75*G6</f>
         <v>58500</v>
       </c>
-      <c r="F6" s="22">
+      <c r="F6" s="20">
         <f>0.9*G6</f>
         <v>70200</v>
       </c>
-      <c r="G6" s="22">
+      <c r="G6" s="20">
         <f>($B$21*$B$25+$B$22*$B$26)</f>
         <v>78000</v>
       </c>
-      <c r="H6" s="22">
+      <c r="H6" s="20">
         <f>($B$21*$B$25+$B$22*$B$26)</f>
         <v>78000</v>
       </c>
-      <c r="I6" s="22">
+      <c r="I6" s="20">
         <f t="shared" ref="I6:N6" si="2">1.05*($B$21*$B$25+$B$22*$B$26)</f>
         <v>81900</v>
       </c>
-      <c r="J6" s="22">
+      <c r="J6" s="20">
         <f t="shared" si="2"/>
         <v>81900</v>
       </c>
-      <c r="K6" s="22">
+      <c r="K6" s="20">
         <f t="shared" si="2"/>
         <v>81900</v>
       </c>
-      <c r="L6" s="22">
+      <c r="L6" s="20">
         <f t="shared" si="2"/>
         <v>81900</v>
       </c>
-      <c r="M6" s="22">
+      <c r="M6" s="20">
         <f t="shared" si="2"/>
         <v>81900</v>
       </c>
-      <c r="N6" s="23">
+      <c r="N6" s="21">
         <f t="shared" si="2"/>
         <v>81900</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="18">
-      <c r="A7" s="20" t="s">
+    <row r="7" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A7" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22">
+      <c r="B7" s="19"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20">
         <f t="shared" ref="E7:N7" si="3">SUM(E8:E10)</f>
         <v>18678.88</v>
       </c>
-      <c r="F7" s="22">
+      <c r="F7" s="20">
         <f t="shared" si="3"/>
         <v>22406.655999999999</v>
       </c>
-      <c r="G7" s="22">
+      <c r="G7" s="20">
         <f t="shared" si="3"/>
         <v>24891.84</v>
       </c>
-      <c r="H7" s="22">
+      <c r="H7" s="20">
         <f t="shared" si="3"/>
         <v>29870.207999999999</v>
       </c>
-      <c r="I7" s="22">
+      <c r="I7" s="20">
         <f t="shared" si="3"/>
         <v>29870.207999999999</v>
       </c>
-      <c r="J7" s="22">
+      <c r="J7" s="20">
         <f t="shared" si="3"/>
         <v>29870.207999999999</v>
       </c>
-      <c r="K7" s="22">
+      <c r="K7" s="20">
         <f t="shared" si="3"/>
         <v>29870.207999999999</v>
       </c>
-      <c r="L7" s="22">
+      <c r="L7" s="20">
         <f t="shared" si="3"/>
         <v>29870.207999999999</v>
       </c>
-      <c r="M7" s="22">
+      <c r="M7" s="20">
         <f t="shared" si="3"/>
         <v>29870.207999999999</v>
       </c>
-      <c r="N7" s="23">
+      <c r="N7" s="21">
         <f t="shared" si="3"/>
         <v>29870.207999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="18">
-      <c r="A8" s="20" t="s">
+    <row r="8" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A8" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22">
+      <c r="B8" s="19"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20">
         <v>40</v>
       </c>
-      <c r="F8" s="22">
+      <c r="F8" s="20">
         <v>40</v>
       </c>
-      <c r="G8" s="22">
+      <c r="G8" s="20">
         <v>40</v>
       </c>
-      <c r="H8" s="22">
+      <c r="H8" s="20">
         <f t="shared" ref="H8:N8" si="4">$G$8*1.2</f>
         <v>48</v>
       </c>
-      <c r="I8" s="22">
+      <c r="I8" s="20">
         <f t="shared" si="4"/>
         <v>48</v>
       </c>
-      <c r="J8" s="22">
+      <c r="J8" s="20">
         <f t="shared" si="4"/>
         <v>48</v>
       </c>
-      <c r="K8" s="22">
+      <c r="K8" s="20">
         <f t="shared" si="4"/>
         <v>48</v>
       </c>
-      <c r="L8" s="22">
+      <c r="L8" s="20">
         <f t="shared" si="4"/>
         <v>48</v>
       </c>
-      <c r="M8" s="22">
+      <c r="M8" s="20">
         <f t="shared" si="4"/>
         <v>48</v>
       </c>
-      <c r="N8" s="23">
+      <c r="N8" s="21">
         <f t="shared" si="4"/>
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="18">
-      <c r="A9" s="20" t="s">
+    <row r="9" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A9" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22">
+      <c r="B9" s="19"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20">
         <f>0.75*G9</f>
         <v>18450</v>
       </c>
-      <c r="F9" s="22">
+      <c r="F9" s="20">
         <f>0.9*G9</f>
         <v>22140</v>
       </c>
-      <c r="G9" s="22">
+      <c r="G9" s="20">
         <f>($B$23*$B$27)</f>
         <v>24600</v>
       </c>
-      <c r="H9" s="22">
+      <c r="H9" s="20">
         <f>1.2*($B$23*$B$27)</f>
         <v>29520</v>
       </c>
-      <c r="I9" s="22">
+      <c r="I9" s="20">
         <f t="shared" ref="I9:N9" si="5">1.2*($B$23*$B$27)</f>
         <v>29520</v>
       </c>
-      <c r="J9" s="22">
+      <c r="J9" s="20">
         <f t="shared" si="5"/>
         <v>29520</v>
       </c>
-      <c r="K9" s="22">
+      <c r="K9" s="20">
         <f t="shared" si="5"/>
         <v>29520</v>
       </c>
-      <c r="L9" s="22">
+      <c r="L9" s="20">
         <f t="shared" si="5"/>
         <v>29520</v>
       </c>
-      <c r="M9" s="22">
+      <c r="M9" s="20">
         <f t="shared" si="5"/>
         <v>29520</v>
       </c>
-      <c r="N9" s="23">
+      <c r="N9" s="21">
         <f t="shared" si="5"/>
         <v>29520</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="18">
-      <c r="A10" s="20" t="s">
+    <row r="10" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A10" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22">
+      <c r="B10" s="19"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20">
         <f>0.75*G10</f>
         <v>188.88</v>
       </c>
-      <c r="F10" s="22">
+      <c r="F10" s="20">
         <f>0.9*G10</f>
         <v>226.65600000000001</v>
       </c>
-      <c r="G10" s="22">
+      <c r="G10" s="20">
         <f>$D$28+$D$29</f>
         <v>251.84</v>
       </c>
-      <c r="H10" s="22">
+      <c r="H10" s="20">
         <f t="shared" ref="H10:N10" si="6">($D$28+$D$29)*1.2</f>
         <v>302.20799999999997</v>
       </c>
-      <c r="I10" s="22">
+      <c r="I10" s="20">
         <f t="shared" si="6"/>
         <v>302.20799999999997</v>
       </c>
-      <c r="J10" s="22">
+      <c r="J10" s="20">
         <f t="shared" si="6"/>
         <v>302.20799999999997</v>
       </c>
-      <c r="K10" s="22">
+      <c r="K10" s="20">
         <f t="shared" si="6"/>
         <v>302.20799999999997</v>
       </c>
-      <c r="L10" s="22">
+      <c r="L10" s="20">
         <f t="shared" si="6"/>
         <v>302.20799999999997</v>
       </c>
-      <c r="M10" s="22">
+      <c r="M10" s="20">
         <f t="shared" si="6"/>
         <v>302.20799999999997</v>
       </c>
-      <c r="N10" s="23">
+      <c r="N10" s="21">
         <f t="shared" si="6"/>
         <v>302.20799999999997</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="18.75" thickBot="1">
-      <c r="A11" s="24"/>
-      <c r="B11" s="25"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="26"/>
-      <c r="J11" s="26"/>
-      <c r="K11" s="26"/>
-      <c r="L11" s="26"/>
-      <c r="M11" s="26"/>
-      <c r="N11" s="27"/>
-    </row>
-    <row r="12" spans="1:14" s="1" customFormat="1" ht="18.75" thickBot="1">
-      <c r="A12" s="28" t="s">
+    <row r="11" spans="1:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="22"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="24"/>
+      <c r="M11" s="24"/>
+      <c r="N11" s="25"/>
+    </row>
+    <row r="12" spans="1:14" s="1" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="29">
+      <c r="B12" s="27">
         <f t="shared" ref="B12:N12" si="7">SUM(B4+B5+B6-B7)</f>
         <v>-28000</v>
       </c>
-      <c r="C12" s="30">
+      <c r="C12" s="28">
         <f t="shared" si="7"/>
         <v>-70000</v>
       </c>
-      <c r="D12" s="30">
+      <c r="D12" s="28">
         <f t="shared" si="7"/>
         <v>-42000</v>
       </c>
-      <c r="E12" s="30">
+      <c r="E12" s="28">
         <f t="shared" si="7"/>
         <v>35151.399999999994</v>
       </c>
-      <c r="F12" s="30">
+      <c r="F12" s="28">
         <f t="shared" si="7"/>
         <v>46861.399999999994</v>
       </c>
-      <c r="G12" s="30">
+      <c r="G12" s="28">
         <f t="shared" si="7"/>
         <v>52486.864000000001</v>
       </c>
-      <c r="H12" s="30">
+      <c r="H12" s="28">
         <f t="shared" si="7"/>
         <v>46885.2</v>
       </c>
-      <c r="I12" s="30">
+      <c r="I12" s="28">
         <f t="shared" si="7"/>
         <v>52029.792000000001</v>
       </c>
-      <c r="J12" s="30">
+      <c r="J12" s="28">
         <f t="shared" si="7"/>
         <v>52029.792000000001</v>
       </c>
-      <c r="K12" s="30">
+      <c r="K12" s="28">
         <f t="shared" si="7"/>
         <v>52029.792000000001</v>
       </c>
-      <c r="L12" s="30">
+      <c r="L12" s="28">
         <f t="shared" si="7"/>
         <v>52029.792000000001</v>
       </c>
-      <c r="M12" s="30">
+      <c r="M12" s="28">
         <f t="shared" si="7"/>
         <v>52029.792000000001</v>
       </c>
-      <c r="N12" s="31">
+      <c r="N12" s="29">
         <f t="shared" si="7"/>
         <v>59497.343999999997</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="18">
-      <c r="A13" s="16" t="s">
+    <row r="13" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A13" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="32"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33">
+      <c r="B13" s="30"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31">
         <f t="shared" ref="E13:N13" si="8">-SUM($B$4:$D$4)/10</f>
         <v>14000</v>
       </c>
-      <c r="F13" s="33">
+      <c r="F13" s="31">
         <f t="shared" si="8"/>
         <v>14000</v>
       </c>
-      <c r="G13" s="33">
+      <c r="G13" s="31">
         <f t="shared" si="8"/>
         <v>14000</v>
       </c>
-      <c r="H13" s="33">
+      <c r="H13" s="31">
         <f t="shared" si="8"/>
         <v>14000</v>
       </c>
-      <c r="I13" s="33">
+      <c r="I13" s="31">
         <f t="shared" si="8"/>
         <v>14000</v>
       </c>
-      <c r="J13" s="33">
+      <c r="J13" s="31">
         <f t="shared" si="8"/>
         <v>14000</v>
       </c>
-      <c r="K13" s="33">
+      <c r="K13" s="31">
         <f t="shared" si="8"/>
         <v>14000</v>
       </c>
-      <c r="L13" s="33">
+      <c r="L13" s="31">
         <f t="shared" si="8"/>
         <v>14000</v>
       </c>
-      <c r="M13" s="33">
+      <c r="M13" s="31">
         <f t="shared" si="8"/>
         <v>14000</v>
       </c>
-      <c r="N13" s="34">
+      <c r="N13" s="32">
         <f t="shared" si="8"/>
         <v>14000</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="18">
-      <c r="A14" s="20" t="s">
+    <row r="14" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A14" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="21"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22">
+      <c r="B14" s="19"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20">
         <f>0.1*(E6-E7-E13)</f>
         <v>2582.1119999999996</v>
       </c>
-      <c r="F14" s="22">
+      <c r="F14" s="20">
         <f t="shared" ref="F14:N14" si="9">0.1*(F6-F7-F13)</f>
         <v>3379.3343999999997</v>
       </c>
-      <c r="G14" s="22">
+      <c r="G14" s="20">
         <f t="shared" si="9"/>
         <v>3910.8160000000007</v>
       </c>
-      <c r="H14" s="22">
+      <c r="H14" s="20">
         <f t="shared" si="9"/>
         <v>3412.9792000000002</v>
       </c>
-      <c r="I14" s="22">
+      <c r="I14" s="20">
         <f t="shared" si="9"/>
         <v>3802.9792000000002</v>
       </c>
-      <c r="J14" s="22">
+      <c r="J14" s="20">
         <f t="shared" si="9"/>
         <v>3802.9792000000002</v>
       </c>
-      <c r="K14" s="22">
+      <c r="K14" s="20">
         <f t="shared" si="9"/>
         <v>3802.9792000000002</v>
       </c>
-      <c r="L14" s="22">
+      <c r="L14" s="20">
         <f t="shared" si="9"/>
         <v>3802.9792000000002</v>
       </c>
-      <c r="M14" s="22">
+      <c r="M14" s="20">
         <f t="shared" si="9"/>
         <v>3802.9792000000002</v>
       </c>
-      <c r="N14" s="23">
+      <c r="N14" s="21">
         <f t="shared" si="9"/>
         <v>3802.9792000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="18.75" thickBot="1">
-      <c r="A15" s="24"/>
-      <c r="B15" s="25"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="26"/>
-      <c r="K15" s="26"/>
-      <c r="L15" s="26"/>
-      <c r="M15" s="26"/>
-      <c r="N15" s="27"/>
-    </row>
-    <row r="16" spans="1:14" s="1" customFormat="1" ht="18.75" thickBot="1">
-      <c r="A16" s="28" t="s">
+    <row r="15" spans="1:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="22"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="24"/>
+      <c r="K15" s="24"/>
+      <c r="L15" s="24"/>
+      <c r="M15" s="24"/>
+      <c r="N15" s="25"/>
+    </row>
+    <row r="16" spans="1:14" s="1" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="29">
+      <c r="B16" s="27">
         <f t="shared" ref="B16:N16" si="10">B12-B14</f>
         <v>-28000</v>
       </c>
-      <c r="C16" s="30">
+      <c r="C16" s="28">
         <f t="shared" si="10"/>
         <v>-70000</v>
       </c>
-      <c r="D16" s="30">
+      <c r="D16" s="28">
         <f t="shared" si="10"/>
         <v>-42000</v>
       </c>
-      <c r="E16" s="30">
+      <c r="E16" s="28">
         <f t="shared" si="10"/>
         <v>32569.287999999993</v>
       </c>
-      <c r="F16" s="30">
+      <c r="F16" s="28">
         <f t="shared" si="10"/>
         <v>43482.065599999994</v>
       </c>
-      <c r="G16" s="30">
+      <c r="G16" s="28">
         <f t="shared" si="10"/>
         <v>48576.048000000003</v>
       </c>
-      <c r="H16" s="30">
+      <c r="H16" s="28">
         <f t="shared" si="10"/>
         <v>43472.220799999996</v>
       </c>
-      <c r="I16" s="30">
+      <c r="I16" s="28">
         <f t="shared" si="10"/>
         <v>48226.8128</v>
       </c>
-      <c r="J16" s="30">
+      <c r="J16" s="28">
         <f t="shared" si="10"/>
         <v>48226.8128</v>
       </c>
-      <c r="K16" s="30">
+      <c r="K16" s="28">
         <f t="shared" si="10"/>
         <v>48226.8128</v>
       </c>
-      <c r="L16" s="30">
+      <c r="L16" s="28">
         <f t="shared" si="10"/>
         <v>48226.8128</v>
       </c>
-      <c r="M16" s="30">
+      <c r="M16" s="28">
         <f t="shared" si="10"/>
         <v>48226.8128</v>
       </c>
-      <c r="N16" s="31">
+      <c r="N16" s="29">
         <f t="shared" si="10"/>
         <v>55694.364799999996</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="13.5" thickBot="1"/>
-    <row r="18" spans="1:10" ht="18.75" thickBot="1">
-      <c r="A18" s="35" t="s">
+    <row r="17" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="36">
+      <c r="B18" s="34">
         <f>IRR(B16:N16)</f>
-        <v>0.22434040872510433</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="25.5">
-      <c r="A19" s="11" t="s">
+        <v>0.22434040872513239</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="11"/>
+      <c r="B19" s="9"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
-      <c r="I19" s="8" t="s">
+      <c r="I19" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="J19" s="9">
+      <c r="J19" s="7">
         <f>('CASO ABC CASO BASE'!G20-'CASO ABC CASO BASE'!G22)/('CASO ABC CASO BASE'!F22-'CASO ABC CASO BASE'!F20)</f>
-        <v>-1.9580558491587349E-3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10">
+        <v>-1.9580558491605763E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>8</v>
       </c>
@@ -1736,7 +1761,7 @@
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>9</v>
       </c>
@@ -1746,7 +1771,7 @@
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>11</v>
       </c>
@@ -1756,7 +1781,7 @@
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>10</v>
       </c>
@@ -1766,38 +1791,38 @@
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="1:10">
-      <c r="A24" s="11" t="s">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B24" s="11"/>
+      <c r="B24" s="9"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B25" s="10">
+      <c r="B25" s="8">
         <v>90</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
-      <c r="F25" s="10" t="s">
+      <c r="F25" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B26" s="10">
+      <c r="B26" s="8">
         <v>60</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>10</v>
       </c>
@@ -1807,11 +1832,11 @@
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B28" s="10">
+      <c r="B28" s="8">
         <v>22.5</v>
       </c>
       <c r="C28" s="1">
@@ -1822,7 +1847,7 @@
         <v>247.5</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>19</v>
       </c>
@@ -1849,848 +1874,848 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.85546875" customWidth="1"/>
-    <col min="2" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.88671875" customWidth="1"/>
+    <col min="2" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="20.25">
-      <c r="A1" s="78" t="s">
+    <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="76" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="80"/>
-      <c r="I1" s="80"/>
-      <c r="J1" s="80"/>
-      <c r="K1" s="80"/>
-      <c r="L1" s="80"/>
-      <c r="M1" s="80"/>
-      <c r="N1" s="80"/>
-    </row>
-    <row r="2" spans="1:14" ht="13.5" thickBot="1"/>
-    <row r="3" spans="1:14" s="4" customFormat="1" ht="36.75" thickBot="1">
-      <c r="A3" s="40" t="s">
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="78"/>
+      <c r="K1" s="78"/>
+      <c r="L1" s="78"/>
+      <c r="M1" s="78"/>
+      <c r="N1" s="78"/>
+    </row>
+    <row r="2" spans="1:14" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:14" s="4" customFormat="1" ht="35.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="37">
+      <c r="B3" s="35">
         <v>1</v>
       </c>
-      <c r="C3" s="38">
+      <c r="C3" s="36">
         <f t="shared" ref="C3:N3" si="0">B3+1</f>
         <v>2</v>
       </c>
-      <c r="D3" s="38">
+      <c r="D3" s="36">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E3" s="38">
+      <c r="E3" s="36">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="F3" s="38">
+      <c r="F3" s="36">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G3" s="38">
+      <c r="G3" s="36">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="H3" s="38">
+      <c r="H3" s="36">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="I3" s="38">
+      <c r="I3" s="36">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="J3" s="38">
+      <c r="J3" s="36">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="K3" s="38">
+      <c r="K3" s="36">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="L3" s="38">
+      <c r="L3" s="36">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="M3" s="38">
+      <c r="M3" s="36">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="N3" s="39">
+      <c r="N3" s="37">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="18">
-      <c r="A4" s="41" t="s">
+    <row r="4" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A4" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="17">
+      <c r="B4" s="15">
         <f>-0.2*$B$20</f>
         <v>-28000</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="16">
         <f>-0.5*$B$20</f>
         <v>-70000</v>
       </c>
-      <c r="D4" s="18">
+      <c r="D4" s="16">
         <f>-0.3*$B$20</f>
         <v>-42000</v>
       </c>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18"/>
-      <c r="M4" s="18"/>
-      <c r="N4" s="19"/>
-    </row>
-    <row r="5" spans="1:14" ht="18">
-      <c r="A5" s="42" t="s">
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="17"/>
+    </row>
+    <row r="5" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A5" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22">
+      <c r="B5" s="19"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20">
         <f>-E7*(3/12)</f>
         <v>-4669.72</v>
       </c>
-      <c r="F5" s="22">
+      <c r="F5" s="20">
         <f>-F7*(3/12)+E7*(3/12)</f>
         <v>-931.94399999999951</v>
       </c>
-      <c r="G5" s="22">
+      <c r="G5" s="20">
         <f>-G7*(3/12)+F7*(3/12)</f>
         <v>-621.29600000000028</v>
       </c>
-      <c r="H5" s="22">
+      <c r="H5" s="20">
         <f t="shared" ref="H5:M5" si="1">-H7*(3/12)+G7*(3/12)</f>
         <v>-1244.5919999999996</v>
       </c>
-      <c r="I5" s="22">
+      <c r="I5" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J5" s="22">
+      <c r="J5" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K5" s="22">
+      <c r="K5" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L5" s="22">
+      <c r="L5" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M5" s="22">
+      <c r="M5" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N5" s="23">
+      <c r="N5" s="21">
         <f>SUM(E5:M5)*-1</f>
         <v>7467.5519999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="18">
-      <c r="A6" s="42" t="s">
+    <row r="6" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A6" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22">
+      <c r="B6" s="19"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20">
         <f>0.75*G6</f>
         <v>58500</v>
       </c>
-      <c r="F6" s="22">
+      <c r="F6" s="20">
         <f>0.9*G6</f>
         <v>70200</v>
       </c>
-      <c r="G6" s="22">
+      <c r="G6" s="20">
         <f>($B$21*$B$25+$B$22*$B$26)</f>
         <v>78000</v>
       </c>
-      <c r="H6" s="22">
+      <c r="H6" s="20">
         <f>($B$21*$B$25+$B$22*$B$26)</f>
         <v>78000</v>
       </c>
-      <c r="I6" s="22">
+      <c r="I6" s="20">
         <f t="shared" ref="I6:N6" si="2">1.05*($B$21*$B$25+$B$22*$B$26)</f>
         <v>81900</v>
       </c>
-      <c r="J6" s="22">
+      <c r="J6" s="20">
         <f t="shared" si="2"/>
         <v>81900</v>
       </c>
-      <c r="K6" s="22">
+      <c r="K6" s="20">
         <f t="shared" si="2"/>
         <v>81900</v>
       </c>
-      <c r="L6" s="22">
+      <c r="L6" s="20">
         <f t="shared" si="2"/>
         <v>81900</v>
       </c>
-      <c r="M6" s="22">
+      <c r="M6" s="20">
         <f t="shared" si="2"/>
         <v>81900</v>
       </c>
-      <c r="N6" s="23">
+      <c r="N6" s="21">
         <f t="shared" si="2"/>
         <v>81900</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="18">
-      <c r="A7" s="42" t="s">
+    <row r="7" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A7" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22">
+      <c r="B7" s="19"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20">
         <f t="shared" ref="E7:N7" si="3">SUM(E8:E10)</f>
         <v>18678.88</v>
       </c>
-      <c r="F7" s="22">
+      <c r="F7" s="20">
         <f t="shared" si="3"/>
         <v>22406.655999999999</v>
       </c>
-      <c r="G7" s="22">
+      <c r="G7" s="20">
         <f t="shared" si="3"/>
         <v>24891.84</v>
       </c>
-      <c r="H7" s="22">
+      <c r="H7" s="20">
         <f t="shared" si="3"/>
         <v>29870.207999999999</v>
       </c>
-      <c r="I7" s="22">
+      <c r="I7" s="20">
         <f t="shared" si="3"/>
         <v>29870.207999999999</v>
       </c>
-      <c r="J7" s="22">
+      <c r="J7" s="20">
         <f t="shared" si="3"/>
         <v>29870.207999999999</v>
       </c>
-      <c r="K7" s="22">
+      <c r="K7" s="20">
         <f t="shared" si="3"/>
         <v>29870.207999999999</v>
       </c>
-      <c r="L7" s="22">
+      <c r="L7" s="20">
         <f t="shared" si="3"/>
         <v>29870.207999999999</v>
       </c>
-      <c r="M7" s="22">
+      <c r="M7" s="20">
         <f t="shared" si="3"/>
         <v>29870.207999999999</v>
       </c>
-      <c r="N7" s="23">
+      <c r="N7" s="21">
         <f t="shared" si="3"/>
         <v>29870.207999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="18">
-      <c r="A8" s="42" t="s">
+    <row r="8" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A8" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22">
+      <c r="B8" s="19"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20">
         <v>40</v>
       </c>
-      <c r="F8" s="22">
+      <c r="F8" s="20">
         <v>40</v>
       </c>
-      <c r="G8" s="22">
+      <c r="G8" s="20">
         <v>40</v>
       </c>
-      <c r="H8" s="22">
+      <c r="H8" s="20">
+        <f>$G$8*1.2</f>
+        <v>48</v>
+      </c>
+      <c r="I8" s="20">
         <f t="shared" ref="H8:N8" si="4">$G$8*1.2</f>
         <v>48</v>
       </c>
-      <c r="I8" s="22">
+      <c r="J8" s="20">
         <f t="shared" si="4"/>
         <v>48</v>
       </c>
-      <c r="J8" s="22">
+      <c r="K8" s="20">
         <f t="shared" si="4"/>
         <v>48</v>
       </c>
-      <c r="K8" s="22">
+      <c r="L8" s="20">
         <f t="shared" si="4"/>
         <v>48</v>
       </c>
-      <c r="L8" s="22">
+      <c r="M8" s="20">
         <f t="shared" si="4"/>
         <v>48</v>
       </c>
-      <c r="M8" s="22">
+      <c r="N8" s="21">
         <f t="shared" si="4"/>
         <v>48</v>
       </c>
-      <c r="N8" s="23">
-        <f t="shared" si="4"/>
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="18">
-      <c r="A9" s="42" t="s">
+    </row>
+    <row r="9" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A9" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22">
+      <c r="B9" s="19"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20">
         <f>0.75*G9</f>
         <v>18450</v>
       </c>
-      <c r="F9" s="22">
+      <c r="F9" s="20">
         <f>0.9*G9</f>
         <v>22140</v>
       </c>
-      <c r="G9" s="22">
+      <c r="G9" s="20">
         <f>($B$23*$B$27)</f>
         <v>24600</v>
       </c>
-      <c r="H9" s="22">
+      <c r="H9" s="20">
         <f>1.2*($B$23*$B$27)</f>
         <v>29520</v>
       </c>
-      <c r="I9" s="22">
+      <c r="I9" s="20">
         <f t="shared" ref="I9:N9" si="5">1.2*($B$23*$B$27)</f>
         <v>29520</v>
       </c>
-      <c r="J9" s="22">
+      <c r="J9" s="20">
         <f t="shared" si="5"/>
         <v>29520</v>
       </c>
-      <c r="K9" s="22">
+      <c r="K9" s="20">
         <f t="shared" si="5"/>
         <v>29520</v>
       </c>
-      <c r="L9" s="22">
+      <c r="L9" s="20">
         <f t="shared" si="5"/>
         <v>29520</v>
       </c>
-      <c r="M9" s="22">
+      <c r="M9" s="20">
         <f t="shared" si="5"/>
         <v>29520</v>
       </c>
-      <c r="N9" s="23">
+      <c r="N9" s="21">
         <f t="shared" si="5"/>
         <v>29520</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="18">
-      <c r="A10" s="42" t="s">
+    <row r="10" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A10" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22">
+      <c r="B10" s="19"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20">
         <f>0.75*G10</f>
         <v>188.88</v>
       </c>
-      <c r="F10" s="22">
+      <c r="F10" s="20">
         <f>0.9*G10</f>
         <v>226.65600000000001</v>
       </c>
-      <c r="G10" s="22">
+      <c r="G10" s="20">
         <f>$D$28+$D$29</f>
         <v>251.84</v>
       </c>
-      <c r="H10" s="22">
+      <c r="H10" s="20">
         <f t="shared" ref="H10:N10" si="6">($D$28+$D$29)*1.2</f>
         <v>302.20799999999997</v>
       </c>
-      <c r="I10" s="22">
+      <c r="I10" s="20">
         <f t="shared" si="6"/>
         <v>302.20799999999997</v>
       </c>
-      <c r="J10" s="22">
+      <c r="J10" s="20">
         <f t="shared" si="6"/>
         <v>302.20799999999997</v>
       </c>
-      <c r="K10" s="22">
+      <c r="K10" s="20">
         <f t="shared" si="6"/>
         <v>302.20799999999997</v>
       </c>
-      <c r="L10" s="22">
+      <c r="L10" s="20">
         <f t="shared" si="6"/>
         <v>302.20799999999997</v>
       </c>
-      <c r="M10" s="22">
+      <c r="M10" s="20">
         <f t="shared" si="6"/>
         <v>302.20799999999997</v>
       </c>
-      <c r="N10" s="23">
+      <c r="N10" s="21">
         <f t="shared" si="6"/>
         <v>302.20799999999997</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="18.75" thickBot="1">
-      <c r="A11" s="43"/>
-      <c r="B11" s="25"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="26"/>
-      <c r="J11" s="26"/>
-      <c r="K11" s="26"/>
-      <c r="L11" s="26"/>
-      <c r="M11" s="26"/>
-      <c r="N11" s="27"/>
-    </row>
-    <row r="12" spans="1:14" s="1" customFormat="1" ht="18.75" thickBot="1">
-      <c r="A12" s="44" t="s">
+    <row r="11" spans="1:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="41"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="24"/>
+      <c r="M11" s="24"/>
+      <c r="N11" s="25"/>
+    </row>
+    <row r="12" spans="1:14" s="1" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="29">
+      <c r="B12" s="27">
         <f t="shared" ref="B12:N12" si="7">SUM(B4+B5+B6-B7)</f>
         <v>-28000</v>
       </c>
-      <c r="C12" s="30">
+      <c r="C12" s="28">
         <f t="shared" si="7"/>
         <v>-70000</v>
       </c>
-      <c r="D12" s="30">
+      <c r="D12" s="28">
         <f t="shared" si="7"/>
         <v>-42000</v>
       </c>
-      <c r="E12" s="30">
-        <f t="shared" si="7"/>
+      <c r="E12" s="28">
+        <f>SUM(E4+E5+E6-E7)</f>
         <v>35151.399999999994</v>
       </c>
-      <c r="F12" s="30">
+      <c r="F12" s="28">
         <f t="shared" si="7"/>
         <v>46861.399999999994</v>
       </c>
-      <c r="G12" s="30">
-        <f t="shared" si="7"/>
+      <c r="G12" s="28">
+        <f>SUM(G4+G5+G6-G7)</f>
         <v>52486.864000000001</v>
       </c>
-      <c r="H12" s="30">
+      <c r="H12" s="28">
         <f t="shared" si="7"/>
         <v>46885.2</v>
       </c>
-      <c r="I12" s="30">
+      <c r="I12" s="28">
         <f t="shared" si="7"/>
         <v>52029.792000000001</v>
       </c>
-      <c r="J12" s="30">
+      <c r="J12" s="28">
         <f t="shared" si="7"/>
         <v>52029.792000000001</v>
       </c>
-      <c r="K12" s="30">
+      <c r="K12" s="28">
         <f t="shared" si="7"/>
         <v>52029.792000000001</v>
       </c>
-      <c r="L12" s="30">
+      <c r="L12" s="28">
         <f t="shared" si="7"/>
         <v>52029.792000000001</v>
       </c>
-      <c r="M12" s="30">
+      <c r="M12" s="28">
         <f t="shared" si="7"/>
         <v>52029.792000000001</v>
       </c>
-      <c r="N12" s="31">
+      <c r="N12" s="29">
         <f t="shared" si="7"/>
         <v>59497.343999999997</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="18">
-      <c r="A13" s="41" t="s">
+    <row r="13" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A13" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="32"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33">
+      <c r="B13" s="30"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31">
+        <f>-SUM($B$4:$D$4)/10</f>
+        <v>14000</v>
+      </c>
+      <c r="F13" s="31">
         <f t="shared" ref="E13:N13" si="8">-SUM($B$4:$D$4)/10</f>
         <v>14000</v>
       </c>
-      <c r="F13" s="33">
+      <c r="G13" s="31">
+        <f>-SUM($B$4:$D$4)/10</f>
+        <v>14000</v>
+      </c>
+      <c r="H13" s="31">
         <f t="shared" si="8"/>
         <v>14000</v>
       </c>
-      <c r="G13" s="33">
+      <c r="I13" s="31">
         <f t="shared" si="8"/>
         <v>14000</v>
       </c>
-      <c r="H13" s="33">
+      <c r="J13" s="31">
         <f t="shared" si="8"/>
         <v>14000</v>
       </c>
-      <c r="I13" s="33">
+      <c r="K13" s="31">
         <f t="shared" si="8"/>
         <v>14000</v>
       </c>
-      <c r="J13" s="33">
+      <c r="L13" s="31">
         <f t="shared" si="8"/>
         <v>14000</v>
       </c>
-      <c r="K13" s="33">
+      <c r="M13" s="31">
         <f t="shared" si="8"/>
         <v>14000</v>
       </c>
-      <c r="L13" s="33">
+      <c r="N13" s="32">
         <f t="shared" si="8"/>
         <v>14000</v>
       </c>
-      <c r="M13" s="33">
-        <f t="shared" si="8"/>
-        <v>14000</v>
-      </c>
-      <c r="N13" s="34">
-        <f t="shared" si="8"/>
-        <v>14000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" ht="18">
-      <c r="A14" s="42" t="s">
+    </row>
+    <row r="14" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A14" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="21"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22">
+      <c r="B14" s="19"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20">
         <f>0.36*(E6-E7-E13)</f>
         <v>9295.6031999999977</v>
       </c>
-      <c r="F14" s="22">
+      <c r="F14" s="20">
         <f t="shared" ref="F14:N14" si="9">0.36*(F6-F7-F13)</f>
         <v>12165.603839999998</v>
       </c>
-      <c r="G14" s="22">
-        <f t="shared" si="9"/>
+      <c r="G14" s="20">
+        <f>0.36*(G6-G7-G13)</f>
         <v>14078.937600000001</v>
       </c>
-      <c r="H14" s="22">
+      <c r="H14" s="20">
         <f t="shared" si="9"/>
         <v>12286.725119999999</v>
       </c>
-      <c r="I14" s="22">
+      <c r="I14" s="20">
         <f t="shared" si="9"/>
         <v>13690.725119999999</v>
       </c>
-      <c r="J14" s="22">
+      <c r="J14" s="20">
         <f t="shared" si="9"/>
         <v>13690.725119999999</v>
       </c>
-      <c r="K14" s="22">
+      <c r="K14" s="20">
         <f t="shared" si="9"/>
         <v>13690.725119999999</v>
       </c>
-      <c r="L14" s="22">
+      <c r="L14" s="20">
         <f t="shared" si="9"/>
         <v>13690.725119999999</v>
       </c>
-      <c r="M14" s="22">
+      <c r="M14" s="20">
         <f t="shared" si="9"/>
         <v>13690.725119999999</v>
       </c>
-      <c r="N14" s="22">
+      <c r="N14" s="20">
         <f t="shared" si="9"/>
         <v>13690.725119999999</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="18.75" thickBot="1">
-      <c r="A15" s="43"/>
-      <c r="B15" s="25"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="26"/>
-      <c r="K15" s="26"/>
-      <c r="L15" s="26"/>
-      <c r="M15" s="26"/>
-      <c r="N15" s="27"/>
-    </row>
-    <row r="16" spans="1:14" s="1" customFormat="1" ht="18.75" thickBot="1">
-      <c r="A16" s="44" t="s">
+    <row r="15" spans="1:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="41"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="24"/>
+      <c r="K15" s="24"/>
+      <c r="L15" s="24"/>
+      <c r="M15" s="24"/>
+      <c r="N15" s="25"/>
+    </row>
+    <row r="16" spans="1:14" s="1" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="29">
+      <c r="B16" s="27">
         <f t="shared" ref="B16:N16" si="10">B12-B14</f>
         <v>-28000</v>
       </c>
-      <c r="C16" s="30">
+      <c r="C16" s="28">
         <f t="shared" si="10"/>
         <v>-70000</v>
       </c>
-      <c r="D16" s="30">
+      <c r="D16" s="28">
         <f t="shared" si="10"/>
         <v>-42000</v>
       </c>
-      <c r="E16" s="30">
-        <f t="shared" si="10"/>
+      <c r="E16" s="28">
+        <f>E12-E14</f>
         <v>25855.796799999996</v>
       </c>
-      <c r="F16" s="30">
+      <c r="F16" s="28">
         <f t="shared" si="10"/>
         <v>34695.796159999998</v>
       </c>
-      <c r="G16" s="30">
-        <f t="shared" si="10"/>
+      <c r="G16" s="28">
+        <f>G12-G14</f>
         <v>38407.926399999997</v>
       </c>
-      <c r="H16" s="30">
+      <c r="H16" s="28">
         <f t="shared" si="10"/>
         <v>34598.474879999994</v>
       </c>
-      <c r="I16" s="30">
+      <c r="I16" s="28">
         <f t="shared" si="10"/>
         <v>38339.066879999998</v>
       </c>
-      <c r="J16" s="30">
+      <c r="J16" s="28">
         <f t="shared" si="10"/>
         <v>38339.066879999998</v>
       </c>
-      <c r="K16" s="30">
+      <c r="K16" s="28">
         <f t="shared" si="10"/>
         <v>38339.066879999998</v>
       </c>
-      <c r="L16" s="30">
+      <c r="L16" s="28">
         <f t="shared" si="10"/>
         <v>38339.066879999998</v>
       </c>
-      <c r="M16" s="30">
+      <c r="M16" s="28">
         <f t="shared" si="10"/>
         <v>38339.066879999998</v>
       </c>
-      <c r="N16" s="31">
+      <c r="N16" s="29">
         <f t="shared" si="10"/>
         <v>45806.618879999995</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="13.5" thickBot="1"/>
-    <row r="18" spans="1:14" ht="18.75" thickBot="1">
-      <c r="A18" s="71" t="s">
+    <row r="17" spans="1:14" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="1:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="69" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="72">
+      <c r="B18" s="70">
         <f>IRR(B16:N16)</f>
-        <v>0.17343095664697722</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" ht="48" thickBot="1">
-      <c r="A19" s="73" t="s">
+        <v>0.1734309566469574</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="47.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="74"/>
-      <c r="C19" s="74"/>
-      <c r="D19" s="74"/>
-      <c r="F19" s="63" t="s">
+      <c r="B19" s="72"/>
+      <c r="C19" s="72"/>
+      <c r="D19" s="72"/>
+      <c r="F19" s="61" t="s">
         <v>22</v>
       </c>
-      <c r="G19" s="64" t="s">
+      <c r="G19" s="62" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="15.75">
-      <c r="A20" s="73" t="s">
+    <row r="20" spans="1:14" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A20" s="71" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="74">
+      <c r="B20" s="72">
         <v>140000</v>
       </c>
-      <c r="C20" s="74"/>
-      <c r="D20" s="74"/>
-      <c r="F20" s="65">
+      <c r="C20" s="72"/>
+      <c r="D20" s="72"/>
+      <c r="F20" s="63">
         <v>10</v>
       </c>
-      <c r="G20" s="68">
+      <c r="G20" s="66">
         <f>B18</f>
-        <v>0.17343095664697722</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" ht="15.75">
-      <c r="A21" s="74" t="s">
+        <v>0.1734309566469574</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A21" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="74">
+      <c r="B21" s="72">
         <v>700</v>
       </c>
-      <c r="C21" s="74"/>
-      <c r="D21" s="74"/>
-      <c r="F21" s="66">
+      <c r="C21" s="72"/>
+      <c r="D21" s="72"/>
+      <c r="F21" s="64">
         <v>30</v>
       </c>
-      <c r="G21" s="69">
+      <c r="G21" s="67">
         <f>'CASO ABC IMPTOS 30%'!B18</f>
         <v>0.18578393378177949</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A22" s="74" t="s">
+    <row r="22" spans="1:14" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="72" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="74">
+      <c r="B22" s="72">
         <v>250</v>
       </c>
-      <c r="C22" s="74"/>
-      <c r="D22" s="74"/>
-      <c r="F22" s="67">
+      <c r="C22" s="72"/>
+      <c r="D22" s="72"/>
+      <c r="F22" s="65">
         <v>36</v>
       </c>
-      <c r="G22" s="70">
+      <c r="G22" s="68">
         <f>'caso abc imptos 10%'!B18</f>
-        <v>0.22434040872510433</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14">
-      <c r="A23" s="74" t="s">
+        <v>0.22434040872513239</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="B23" s="74">
+      <c r="B23" s="72">
         <v>820</v>
       </c>
-      <c r="C23" s="74"/>
-      <c r="D23" s="74"/>
-    </row>
-    <row r="24" spans="1:14">
-      <c r="A24" s="75" t="s">
+      <c r="C23" s="72"/>
+      <c r="D23" s="72"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="73" t="s">
         <v>15</v>
       </c>
-      <c r="B24" s="76"/>
-      <c r="C24" s="74"/>
-      <c r="D24" s="74"/>
-    </row>
-    <row r="25" spans="1:14">
-      <c r="A25" s="74" t="s">
+      <c r="B24" s="74"/>
+      <c r="C24" s="72"/>
+      <c r="D24" s="72"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="B25" s="73">
+      <c r="B25" s="71">
         <v>90</v>
       </c>
-      <c r="C25" s="74"/>
-      <c r="D25" s="74"/>
-      <c r="E25" s="10" t="s">
+      <c r="C25" s="72"/>
+      <c r="D25" s="72"/>
+      <c r="E25" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:14">
-      <c r="A26" s="74" t="s">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" s="72" t="s">
         <v>11</v>
       </c>
-      <c r="B26" s="73">
+      <c r="B26" s="71">
         <v>60</v>
       </c>
-      <c r="C26" s="74"/>
-      <c r="D26" s="74"/>
-    </row>
-    <row r="27" spans="1:14">
-      <c r="A27" s="74" t="s">
+      <c r="C26" s="72"/>
+      <c r="D26" s="72"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="B27" s="74">
+      <c r="B27" s="72">
         <v>30</v>
       </c>
-      <c r="C27" s="74"/>
-      <c r="D27" s="74"/>
-    </row>
-    <row r="28" spans="1:14">
-      <c r="A28" s="74" t="s">
+      <c r="C27" s="72"/>
+      <c r="D27" s="72"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" s="72" t="s">
         <v>18</v>
       </c>
-      <c r="B28" s="10">
+      <c r="B28" s="8">
         <v>22.5</v>
       </c>
-      <c r="C28" s="74">
+      <c r="C28" s="72">
         <v>11</v>
       </c>
-      <c r="D28" s="74">
+      <c r="D28" s="72">
         <f>B28*C28</f>
         <v>247.5</v>
       </c>
     </row>
-    <row r="29" spans="1:14">
-      <c r="A29" s="74" t="s">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" s="72" t="s">
         <v>19</v>
       </c>
-      <c r="B29" s="74">
+      <c r="B29" s="72">
         <v>0.01</v>
       </c>
-      <c r="C29" s="74">
+      <c r="C29" s="72">
         <v>434</v>
       </c>
-      <c r="D29" s="74">
+      <c r="D29" s="72">
         <f>B29*C29</f>
         <v>4.34</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="13.5" thickBot="1">
-      <c r="A30" s="74"/>
-      <c r="B30" s="74"/>
-      <c r="C30" s="74"/>
-      <c r="D30" s="74"/>
-    </row>
-    <row r="31" spans="1:14" ht="18.75" thickBot="1">
-      <c r="B31" s="29">
+    <row r="30" spans="1:14" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="72"/>
+      <c r="B30" s="72"/>
+      <c r="C30" s="72"/>
+      <c r="D30" s="72"/>
+    </row>
+    <row r="31" spans="1:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B31" s="27">
         <v>-28000</v>
       </c>
-      <c r="C31" s="30">
+      <c r="C31" s="28">
         <v>-70000</v>
       </c>
-      <c r="D31" s="30">
+      <c r="D31" s="28">
         <v>-42000</v>
       </c>
-      <c r="E31" s="30">
+      <c r="E31" s="28">
         <v>32526.399999999998</v>
       </c>
-      <c r="F31" s="30">
+      <c r="F31" s="28">
         <v>43711.399999999994</v>
       </c>
-      <c r="G31" s="30">
+      <c r="G31" s="28">
         <v>48986.864000000001</v>
       </c>
-      <c r="H31" s="30">
+      <c r="H31" s="28">
         <v>43385.2</v>
       </c>
-      <c r="I31" s="30">
+      <c r="I31" s="28">
         <v>48354.792000000001</v>
       </c>
-      <c r="J31" s="30">
+      <c r="J31" s="28">
         <v>48354.792000000001</v>
       </c>
-      <c r="K31" s="30">
+      <c r="K31" s="28">
         <v>48354.792000000001</v>
       </c>
-      <c r="L31" s="30">
+      <c r="L31" s="28">
         <v>48354.792000000001</v>
       </c>
-      <c r="M31" s="30">
+      <c r="M31" s="28">
         <v>48354.792000000001</v>
       </c>
-      <c r="N31" s="31">
+      <c r="N31" s="29">
         <v>55822.343999999997</v>
       </c>
     </row>
@@ -2706,703 +2731,684 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:P29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28" customWidth="1"/>
-    <col min="2" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="20.25">
-      <c r="A1" s="78" t="s">
+    <row r="1" spans="1:16" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="76" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="80"/>
-      <c r="I1" s="80"/>
-      <c r="J1" s="80"/>
-      <c r="K1" s="80"/>
-      <c r="L1" s="80"/>
-      <c r="M1" s="80"/>
-      <c r="N1" s="80"/>
-    </row>
-    <row r="2" spans="1:16" ht="13.5" thickBot="1"/>
-    <row r="3" spans="1:16" s="4" customFormat="1" ht="36.75" thickBot="1">
-      <c r="A3" s="40" t="s">
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="78"/>
+      <c r="K1" s="78"/>
+      <c r="L1" s="78"/>
+      <c r="M1" s="78"/>
+      <c r="N1" s="78"/>
+    </row>
+    <row r="2" spans="1:16" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:16" s="4" customFormat="1" ht="35.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="45">
+      <c r="B3" s="43">
         <v>1</v>
       </c>
-      <c r="C3" s="46">
+      <c r="C3" s="44">
         <f t="shared" ref="C3:N3" si="0">B3+1</f>
         <v>2</v>
       </c>
-      <c r="D3" s="46">
+      <c r="D3" s="44">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E3" s="46">
+      <c r="E3" s="44">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="F3" s="46">
+      <c r="F3" s="44">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G3" s="46">
+      <c r="G3" s="44">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="H3" s="46">
+      <c r="H3" s="44">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="I3" s="46">
+      <c r="I3" s="44">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="J3" s="46">
+      <c r="J3" s="44">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="K3" s="46">
+      <c r="K3" s="44">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="L3" s="46">
+      <c r="L3" s="44">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="M3" s="46">
+      <c r="M3" s="44">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="N3" s="47">
+      <c r="N3" s="45">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="P3" s="77"/>
-    </row>
-    <row r="4" spans="1:16" ht="18">
-      <c r="A4" s="41" t="s">
+      <c r="P3" s="75"/>
+    </row>
+    <row r="4" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A4" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="48">
+      <c r="B4" s="46">
         <f>-0.2*$B$20</f>
         <v>-28000</v>
       </c>
-      <c r="C4" s="49">
+      <c r="C4" s="47">
         <f>-0.5*$B$20</f>
         <v>-70000</v>
       </c>
-      <c r="D4" s="49">
+      <c r="D4" s="47">
         <f>-0.3*$B$20</f>
         <v>-42000</v>
       </c>
-      <c r="E4" s="49"/>
-      <c r="F4" s="49"/>
-      <c r="G4" s="49"/>
-      <c r="H4" s="49"/>
-      <c r="I4" s="49"/>
-      <c r="J4" s="49"/>
-      <c r="K4" s="49"/>
-      <c r="L4" s="49"/>
-      <c r="M4" s="49"/>
-      <c r="N4" s="50"/>
-    </row>
-    <row r="5" spans="1:16" ht="18">
-      <c r="A5" s="42" t="s">
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
+      <c r="K4" s="47"/>
+      <c r="L4" s="47"/>
+      <c r="M4" s="47"/>
+      <c r="N4" s="48"/>
+    </row>
+    <row r="5" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A5" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="51"/>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52">
+      <c r="B5" s="49"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50">
         <f>-E7*(3/12)</f>
         <v>-4669.72</v>
       </c>
-      <c r="F5" s="52">
+      <c r="F5" s="50">
         <f>-F7*(3/12)+E7*(3/12)</f>
         <v>-931.94399999999951</v>
       </c>
-      <c r="G5" s="52">
+      <c r="G5" s="50">
         <f>-G7*(3/12)+F7*(3/12)</f>
         <v>-621.29600000000028</v>
       </c>
-      <c r="H5" s="52">
+      <c r="H5" s="50">
         <f t="shared" ref="H5:M5" si="1">-H7*(3/12)+G7*(3/12)</f>
         <v>-1244.5919999999996</v>
       </c>
-      <c r="I5" s="52">
+      <c r="I5" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J5" s="52">
+      <c r="J5" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K5" s="52">
+      <c r="K5" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L5" s="52">
+      <c r="L5" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M5" s="52">
+      <c r="M5" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N5" s="53">
+      <c r="N5" s="51">
         <f>SUM(E5:M5)*-1</f>
         <v>7467.5519999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="18">
-      <c r="A6" s="42" t="s">
+    <row r="6" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A6" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="51"/>
-      <c r="C6" s="52"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52">
+      <c r="B6" s="49"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="50">
         <f>0.75*G6</f>
         <v>58500</v>
       </c>
-      <c r="F6" s="52">
+      <c r="F6" s="50">
         <f>0.9*G6</f>
         <v>70200</v>
       </c>
-      <c r="G6" s="52">
+      <c r="G6" s="50">
         <f>($B$21*$B$25+$B$22*$B$26)</f>
         <v>78000</v>
       </c>
-      <c r="H6" s="52">
+      <c r="H6" s="50">
         <f>($B$21*$B$25+$B$22*$B$26)</f>
         <v>78000</v>
       </c>
-      <c r="I6" s="52">
+      <c r="I6" s="50">
+        <f>1.05*($B$21*$B$25+$B$22*$B$26)</f>
+        <v>81900</v>
+      </c>
+      <c r="J6" s="50">
         <f t="shared" ref="I6:N6" si="2">1.05*($B$21*$B$25+$B$22*$B$26)</f>
         <v>81900</v>
       </c>
-      <c r="J6" s="52">
+      <c r="K6" s="50">
         <f t="shared" si="2"/>
         <v>81900</v>
       </c>
-      <c r="K6" s="52">
+      <c r="L6" s="50">
         <f t="shared" si="2"/>
         <v>81900</v>
       </c>
-      <c r="L6" s="52">
+      <c r="M6" s="50">
         <f t="shared" si="2"/>
         <v>81900</v>
       </c>
-      <c r="M6" s="52">
+      <c r="N6" s="51">
         <f t="shared" si="2"/>
         <v>81900</v>
       </c>
-      <c r="N6" s="53">
-        <f t="shared" si="2"/>
-        <v>81900</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" ht="18">
-      <c r="A7" s="42" t="s">
+    </row>
+    <row r="7" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A7" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="51"/>
-      <c r="C7" s="52"/>
-      <c r="D7" s="52"/>
-      <c r="E7" s="52">
-        <f t="shared" ref="E7:N7" si="3">SUM(E8:E10)</f>
+      <c r="B7" s="49"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="50">
+        <f>SUM(E8:E10)</f>
         <v>18678.88</v>
       </c>
-      <c r="F7" s="52">
-        <f t="shared" si="3"/>
+      <c r="F7" s="50">
+        <f t="shared" ref="E7:N7" si="3">SUM(F8:F10)</f>
         <v>22406.655999999999</v>
       </c>
-      <c r="G7" s="52">
+      <c r="G7" s="50">
         <f t="shared" si="3"/>
         <v>24891.84</v>
       </c>
-      <c r="H7" s="52">
+      <c r="H7" s="50">
         <f t="shared" si="3"/>
         <v>29870.207999999999</v>
       </c>
-      <c r="I7" s="52">
+      <c r="I7" s="50">
         <f t="shared" si="3"/>
         <v>29870.207999999999</v>
       </c>
-      <c r="J7" s="52">
+      <c r="J7" s="50">
         <f t="shared" si="3"/>
         <v>29870.207999999999</v>
       </c>
-      <c r="K7" s="52">
+      <c r="K7" s="50">
         <f t="shared" si="3"/>
         <v>29870.207999999999</v>
       </c>
-      <c r="L7" s="52">
+      <c r="L7" s="50">
         <f t="shared" si="3"/>
         <v>29870.207999999999</v>
       </c>
-      <c r="M7" s="52">
+      <c r="M7" s="50">
         <f t="shared" si="3"/>
         <v>29870.207999999999</v>
       </c>
-      <c r="N7" s="53">
+      <c r="N7" s="51">
         <f t="shared" si="3"/>
         <v>29870.207999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="18">
-      <c r="A8" s="42" t="s">
+    <row r="8" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A8" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="51"/>
-      <c r="C8" s="52"/>
-      <c r="D8" s="52"/>
-      <c r="E8" s="52">
+      <c r="B8" s="49"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="50">
         <v>40</v>
       </c>
-      <c r="F8" s="52">
+      <c r="F8" s="50">
         <v>40</v>
       </c>
-      <c r="G8" s="52">
+      <c r="G8" s="50">
         <v>40</v>
       </c>
-      <c r="H8" s="52">
+      <c r="H8" s="50">
         <f t="shared" ref="H8:N8" si="4">$G$8*1.2</f>
         <v>48</v>
       </c>
-      <c r="I8" s="52">
+      <c r="I8" s="50">
         <f t="shared" si="4"/>
         <v>48</v>
       </c>
-      <c r="J8" s="52">
+      <c r="J8" s="50">
         <f t="shared" si="4"/>
         <v>48</v>
       </c>
-      <c r="K8" s="52">
+      <c r="K8" s="50">
         <f t="shared" si="4"/>
         <v>48</v>
       </c>
-      <c r="L8" s="52">
+      <c r="L8" s="50">
         <f t="shared" si="4"/>
         <v>48</v>
       </c>
-      <c r="M8" s="52">
+      <c r="M8" s="50">
         <f t="shared" si="4"/>
         <v>48</v>
       </c>
-      <c r="N8" s="53">
+      <c r="N8" s="51">
         <f t="shared" si="4"/>
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="18">
-      <c r="A9" s="42" t="s">
+    <row r="9" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A9" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="51"/>
-      <c r="C9" s="52"/>
-      <c r="D9" s="52"/>
-      <c r="E9" s="52">
+      <c r="B9" s="49"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="50">
         <f>0.75*G9</f>
         <v>18450</v>
       </c>
-      <c r="F9" s="52">
+      <c r="F9" s="50">
         <f>0.9*G9</f>
         <v>22140</v>
       </c>
-      <c r="G9" s="52">
+      <c r="G9" s="50">
         <f>($B$23*$B$27)</f>
         <v>24600</v>
       </c>
-      <c r="H9" s="52">
+      <c r="H9" s="50">
         <f>1.2*($B$23*$B$27)</f>
         <v>29520</v>
       </c>
-      <c r="I9" s="52">
+      <c r="I9" s="50">
         <f t="shared" ref="I9:N9" si="5">1.2*($B$23*$B$27)</f>
         <v>29520</v>
       </c>
-      <c r="J9" s="52">
+      <c r="J9" s="50">
         <f t="shared" si="5"/>
         <v>29520</v>
       </c>
-      <c r="K9" s="52">
+      <c r="K9" s="50">
         <f t="shared" si="5"/>
         <v>29520</v>
       </c>
-      <c r="L9" s="52">
+      <c r="L9" s="50">
         <f t="shared" si="5"/>
         <v>29520</v>
       </c>
-      <c r="M9" s="52">
+      <c r="M9" s="50">
         <f t="shared" si="5"/>
         <v>29520</v>
       </c>
-      <c r="N9" s="53">
-        <f t="shared" si="5"/>
+      <c r="N9" s="51">
+        <f>1.2*($B$23*$B$27)</f>
         <v>29520</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="18">
-      <c r="A10" s="42" t="s">
+    <row r="10" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A10" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="51"/>
-      <c r="C10" s="52"/>
-      <c r="D10" s="52"/>
-      <c r="E10" s="52">
+      <c r="B10" s="49"/>
+      <c r="C10" s="50"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="50">
         <f>0.75*G10</f>
         <v>188.88</v>
       </c>
-      <c r="F10" s="52">
+      <c r="F10" s="50">
         <f>0.9*G10</f>
         <v>226.65600000000001</v>
       </c>
-      <c r="G10" s="52">
+      <c r="G10" s="50">
         <f>$D$28+$D$29</f>
         <v>251.84</v>
       </c>
-      <c r="H10" s="52">
+      <c r="H10" s="50">
         <f t="shared" ref="H10:N10" si="6">($D$28+$D$29)*1.2</f>
         <v>302.20799999999997</v>
       </c>
-      <c r="I10" s="52">
+      <c r="I10" s="50">
         <f t="shared" si="6"/>
         <v>302.20799999999997</v>
       </c>
-      <c r="J10" s="52">
+      <c r="J10" s="50">
         <f t="shared" si="6"/>
         <v>302.20799999999997</v>
       </c>
-      <c r="K10" s="52">
+      <c r="K10" s="50">
         <f t="shared" si="6"/>
         <v>302.20799999999997</v>
       </c>
-      <c r="L10" s="52">
+      <c r="L10" s="50">
         <f t="shared" si="6"/>
         <v>302.20799999999997</v>
       </c>
-      <c r="M10" s="52">
+      <c r="M10" s="50">
         <f t="shared" si="6"/>
         <v>302.20799999999997</v>
       </c>
-      <c r="N10" s="53">
+      <c r="N10" s="51">
         <f t="shared" si="6"/>
         <v>302.20799999999997</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="18.75" thickBot="1">
-      <c r="A11" s="42"/>
-      <c r="B11" s="54"/>
-      <c r="C11" s="55"/>
-      <c r="D11" s="55"/>
-      <c r="E11" s="55"/>
-      <c r="F11" s="55"/>
-      <c r="G11" s="55"/>
-      <c r="H11" s="55"/>
-      <c r="I11" s="55"/>
-      <c r="J11" s="55"/>
-      <c r="K11" s="55"/>
-      <c r="L11" s="55"/>
-      <c r="M11" s="55"/>
-      <c r="N11" s="56"/>
-    </row>
-    <row r="12" spans="1:16" s="1" customFormat="1" ht="18.75" thickBot="1">
-      <c r="A12" s="42" t="s">
+    <row r="11" spans="1:16" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="40"/>
+      <c r="B11" s="52"/>
+      <c r="C11" s="53"/>
+      <c r="D11" s="53"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="53"/>
+      <c r="G11" s="53"/>
+      <c r="H11" s="53"/>
+      <c r="I11" s="53"/>
+      <c r="J11" s="53"/>
+      <c r="K11" s="53"/>
+      <c r="L11" s="53"/>
+      <c r="M11" s="53"/>
+      <c r="N11" s="54"/>
+    </row>
+    <row r="12" spans="1:16" s="1" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="57">
+      <c r="B12" s="55">
         <f t="shared" ref="B12:N12" si="7">SUM(B4+B5+B6-B7)</f>
         <v>-28000</v>
       </c>
-      <c r="C12" s="58">
+      <c r="C12" s="56">
         <f t="shared" si="7"/>
         <v>-70000</v>
       </c>
-      <c r="D12" s="58">
+      <c r="D12" s="56">
         <f t="shared" si="7"/>
         <v>-42000</v>
       </c>
-      <c r="E12" s="58">
+      <c r="E12" s="56">
         <f t="shared" si="7"/>
         <v>35151.399999999994</v>
       </c>
-      <c r="F12" s="58">
+      <c r="F12" s="56">
         <f t="shared" si="7"/>
         <v>46861.399999999994</v>
       </c>
-      <c r="G12" s="58">
+      <c r="G12" s="56">
         <f t="shared" si="7"/>
         <v>52486.864000000001</v>
       </c>
-      <c r="H12" s="58">
+      <c r="H12" s="56">
         <f t="shared" si="7"/>
         <v>46885.2</v>
       </c>
-      <c r="I12" s="58">
+      <c r="I12" s="56">
         <f t="shared" si="7"/>
         <v>52029.792000000001</v>
       </c>
-      <c r="J12" s="58">
+      <c r="J12" s="56">
         <f t="shared" si="7"/>
         <v>52029.792000000001</v>
       </c>
-      <c r="K12" s="58">
+      <c r="K12" s="56">
         <f t="shared" si="7"/>
         <v>52029.792000000001</v>
       </c>
-      <c r="L12" s="58">
+      <c r="L12" s="56">
         <f t="shared" si="7"/>
         <v>52029.792000000001</v>
       </c>
-      <c r="M12" s="58">
+      <c r="M12" s="56">
         <f t="shared" si="7"/>
         <v>52029.792000000001</v>
       </c>
-      <c r="N12" s="59">
+      <c r="N12" s="57">
         <f t="shared" si="7"/>
         <v>59497.343999999997</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="18">
-      <c r="A13" s="42" t="s">
+    <row r="13" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A13" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="60"/>
-      <c r="C13" s="61"/>
-      <c r="D13" s="61"/>
-      <c r="E13" s="61">
+      <c r="B13" s="58"/>
+      <c r="C13" s="59"/>
+      <c r="D13" s="59"/>
+      <c r="E13" s="59">
+        <f>-SUM($B$4:$D$4)/10</f>
+        <v>14000</v>
+      </c>
+      <c r="F13" s="59">
         <f t="shared" ref="E13:N13" si="8">-SUM($B$4:$D$4)/10</f>
         <v>14000</v>
       </c>
-      <c r="F13" s="61">
+      <c r="G13" s="59">
+        <f>-SUM($B$4:$D$4)/10</f>
+        <v>14000</v>
+      </c>
+      <c r="H13" s="59">
         <f t="shared" si="8"/>
         <v>14000</v>
       </c>
-      <c r="G13" s="61">
+      <c r="I13" s="59">
         <f t="shared" si="8"/>
         <v>14000</v>
       </c>
-      <c r="H13" s="61">
+      <c r="J13" s="59">
         <f t="shared" si="8"/>
         <v>14000</v>
       </c>
-      <c r="I13" s="61">
+      <c r="K13" s="59">
         <f t="shared" si="8"/>
         <v>14000</v>
       </c>
-      <c r="J13" s="61">
+      <c r="L13" s="59">
         <f t="shared" si="8"/>
         <v>14000</v>
       </c>
-      <c r="K13" s="61">
+      <c r="M13" s="59">
         <f t="shared" si="8"/>
         <v>14000</v>
       </c>
-      <c r="L13" s="61">
+      <c r="N13" s="60">
         <f t="shared" si="8"/>
         <v>14000</v>
       </c>
-      <c r="M13" s="61">
-        <f t="shared" si="8"/>
-        <v>14000</v>
-      </c>
-      <c r="N13" s="62">
-        <f t="shared" si="8"/>
-        <v>14000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" ht="18">
-      <c r="A14" s="42" t="s">
+    </row>
+    <row r="14" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A14" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="51"/>
-      <c r="C14" s="52"/>
-      <c r="D14" s="52"/>
-      <c r="E14" s="52">
+      <c r="B14" s="49"/>
+      <c r="C14" s="50"/>
+      <c r="D14" s="50"/>
+      <c r="E14" s="50">
         <f>0.3*(E6-E7-E13)</f>
         <v>7746.3359999999984</v>
       </c>
-      <c r="F14" s="52">
+      <c r="F14" s="50">
         <f t="shared" ref="F14:N14" si="9">0.3*(F6-F7-F13)</f>
         <v>10138.003199999999</v>
       </c>
-      <c r="G14" s="52">
+      <c r="G14" s="50">
         <f t="shared" si="9"/>
         <v>11732.448</v>
       </c>
-      <c r="H14" s="52">
+      <c r="H14" s="50">
         <f t="shared" si="9"/>
         <v>10238.937599999999</v>
       </c>
-      <c r="I14" s="52">
+      <c r="I14" s="50">
         <f t="shared" si="9"/>
         <v>11408.937599999999</v>
       </c>
-      <c r="J14" s="52">
+      <c r="J14" s="50">
         <f t="shared" si="9"/>
         <v>11408.937599999999</v>
       </c>
-      <c r="K14" s="52">
+      <c r="K14" s="50">
         <f t="shared" si="9"/>
         <v>11408.937599999999</v>
       </c>
-      <c r="L14" s="52">
+      <c r="L14" s="50">
         <f t="shared" si="9"/>
         <v>11408.937599999999</v>
       </c>
-      <c r="M14" s="52">
+      <c r="M14" s="50">
         <f t="shared" si="9"/>
         <v>11408.937599999999</v>
       </c>
-      <c r="N14" s="53">
+      <c r="N14" s="51">
         <f t="shared" si="9"/>
         <v>11408.937599999999</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="18.75" thickBot="1">
-      <c r="A15" s="43"/>
-      <c r="B15" s="54"/>
-      <c r="C15" s="55"/>
-      <c r="D15" s="55"/>
-      <c r="E15" s="55"/>
-      <c r="F15" s="55"/>
-      <c r="G15" s="55"/>
-      <c r="H15" s="55"/>
-      <c r="I15" s="55"/>
-      <c r="J15" s="55"/>
-      <c r="K15" s="55"/>
-      <c r="L15" s="55"/>
-      <c r="M15" s="55"/>
-      <c r="N15" s="56"/>
-    </row>
-    <row r="16" spans="1:16" s="1" customFormat="1" ht="18.75" thickBot="1">
-      <c r="A16" s="44" t="s">
+    <row r="15" spans="1:16" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="41"/>
+      <c r="B15" s="52"/>
+      <c r="C15" s="53"/>
+      <c r="D15" s="53"/>
+      <c r="E15" s="53"/>
+      <c r="F15" s="53"/>
+      <c r="G15" s="53"/>
+      <c r="H15" s="53"/>
+      <c r="I15" s="53"/>
+      <c r="J15" s="53"/>
+      <c r="K15" s="53"/>
+      <c r="L15" s="53"/>
+      <c r="M15" s="53"/>
+      <c r="N15" s="54"/>
+    </row>
+    <row r="16" spans="1:16" s="1" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="57">
+      <c r="B16" s="55">
         <f t="shared" ref="B16:N16" si="10">B12-B14</f>
         <v>-28000</v>
       </c>
-      <c r="C16" s="58">
+      <c r="C16" s="56">
         <f t="shared" si="10"/>
         <v>-70000</v>
       </c>
-      <c r="D16" s="58">
+      <c r="D16" s="56">
         <f t="shared" si="10"/>
         <v>-42000</v>
       </c>
-      <c r="E16" s="58">
+      <c r="E16" s="56">
         <f t="shared" si="10"/>
         <v>27405.063999999995</v>
       </c>
-      <c r="F16" s="58">
+      <c r="F16" s="56">
         <f t="shared" si="10"/>
         <v>36723.396799999995</v>
       </c>
-      <c r="G16" s="58">
+      <c r="G16" s="56">
         <f t="shared" si="10"/>
         <v>40754.415999999997</v>
       </c>
-      <c r="H16" s="58">
+      <c r="H16" s="56">
         <f t="shared" si="10"/>
         <v>36646.2624</v>
       </c>
-      <c r="I16" s="58">
+      <c r="I16" s="56">
         <f t="shared" si="10"/>
         <v>40620.854400000004</v>
       </c>
-      <c r="J16" s="58">
+      <c r="J16" s="56">
         <f t="shared" si="10"/>
         <v>40620.854400000004</v>
       </c>
-      <c r="K16" s="58">
+      <c r="K16" s="56">
         <f t="shared" si="10"/>
         <v>40620.854400000004</v>
       </c>
-      <c r="L16" s="58">
+      <c r="L16" s="56">
         <f t="shared" si="10"/>
         <v>40620.854400000004</v>
       </c>
-      <c r="M16" s="58">
+      <c r="M16" s="56">
         <f t="shared" si="10"/>
         <v>40620.854400000004</v>
       </c>
-      <c r="N16" s="59">
+      <c r="N16" s="57">
         <f t="shared" si="10"/>
         <v>48088.4064</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="13.5" thickBot="1"/>
-    <row r="18" spans="1:14" ht="18.75" thickBot="1">
-      <c r="A18" s="71" t="s">
+    <row r="17" spans="1:14" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="1:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="69" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="72">
+      <c r="B18" s="70">
         <f>IRR(B16:N16)</f>
         <v>0.18578393378177949</v>
       </c>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
-    </row>
-    <row r="19" spans="1:14">
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="6"/>
-      <c r="M19" s="6"/>
-      <c r="N19" s="6"/>
-    </row>
-    <row r="20" spans="1:14" ht="15.75">
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+    </row>
+    <row r="20" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B20">
         <v>140000</v>
       </c>
-      <c r="E20" s="5"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
-      <c r="N20" s="5"/>
-    </row>
-    <row r="21" spans="1:14" ht="15.75">
+      <c r="F20" s="3"/>
+    </row>
+    <row r="21" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>9</v>
       </c>
@@ -3411,7 +3417,7 @@
       </c>
       <c r="F21" s="3"/>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>11</v>
       </c>
@@ -3419,7 +3425,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="23" spans="1:14">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>10</v>
       </c>
@@ -3427,31 +3433,31 @@
         <v>820</v>
       </c>
     </row>
-    <row r="24" spans="1:14">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B25" s="10">
+      <c r="B25" s="8">
         <v>90</v>
       </c>
     </row>
-    <row r="26" spans="1:14">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B26" s="10">
+      <c r="B26" s="8">
         <v>60</v>
       </c>
-      <c r="F26" s="10" t="s">
+      <c r="F26" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:14">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>10</v>
       </c>
@@ -3459,11 +3465,11 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:14">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B28" s="10">
+      <c r="B28" s="8">
         <v>22.5</v>
       </c>
       <c r="C28">
@@ -3474,7 +3480,7 @@
         <v>247.5</v>
       </c>
     </row>
-    <row r="29" spans="1:14">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>19</v>
       </c>
@@ -3501,368 +3507,368 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:N29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.7109375" customWidth="1"/>
-    <col min="2" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.6640625" customWidth="1"/>
+    <col min="2" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="20.25">
-      <c r="A1" s="78" t="s">
+    <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="76" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="80"/>
-      <c r="I1" s="80"/>
-      <c r="J1" s="80"/>
-      <c r="K1" s="80"/>
-      <c r="L1" s="80"/>
-      <c r="M1" s="80"/>
-      <c r="N1" s="80"/>
-    </row>
-    <row r="2" spans="1:14" ht="13.5" thickBot="1"/>
-    <row r="3" spans="1:14" s="4" customFormat="1" ht="36.75" thickBot="1">
-      <c r="A3" s="40" t="s">
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="78"/>
+      <c r="K1" s="78"/>
+      <c r="L1" s="78"/>
+      <c r="M1" s="78"/>
+      <c r="N1" s="78"/>
+    </row>
+    <row r="2" spans="1:14" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:14" s="4" customFormat="1" ht="35.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="37">
+      <c r="B3" s="35">
         <v>1</v>
       </c>
-      <c r="C3" s="38">
+      <c r="C3" s="36">
         <f t="shared" ref="C3:N3" si="0">B3+1</f>
         <v>2</v>
       </c>
-      <c r="D3" s="38">
+      <c r="D3" s="36">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E3" s="38">
+      <c r="E3" s="36">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="F3" s="38">
+      <c r="F3" s="36">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G3" s="38">
+      <c r="G3" s="36">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="H3" s="38">
+      <c r="H3" s="36">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="I3" s="38">
+      <c r="I3" s="36">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="J3" s="38">
+      <c r="J3" s="36">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="K3" s="38">
+      <c r="K3" s="36">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="L3" s="38">
+      <c r="L3" s="36">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="M3" s="38">
+      <c r="M3" s="36">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="N3" s="39">
+      <c r="N3" s="37">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="18">
-      <c r="A4" s="41" t="s">
+    <row r="4" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A4" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18"/>
-      <c r="M4" s="18"/>
-      <c r="N4" s="19"/>
-    </row>
-    <row r="5" spans="1:14" ht="18">
-      <c r="A5" s="42" t="s">
+      <c r="B4" s="15"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="17"/>
+    </row>
+    <row r="5" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A5" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="22"/>
-      <c r="J5" s="22"/>
-      <c r="K5" s="22"/>
-      <c r="L5" s="22"/>
-      <c r="M5" s="22"/>
-      <c r="N5" s="23"/>
-    </row>
-    <row r="6" spans="1:14" ht="18">
-      <c r="A6" s="42" t="s">
+      <c r="B5" s="19"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="21"/>
+    </row>
+    <row r="6" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A6" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="22"/>
-      <c r="J6" s="22"/>
-      <c r="K6" s="22"/>
-      <c r="L6" s="22"/>
-      <c r="M6" s="22"/>
-      <c r="N6" s="23"/>
-    </row>
-    <row r="7" spans="1:14" ht="18">
-      <c r="A7" s="42" t="s">
+      <c r="B6" s="19"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="21"/>
+    </row>
+    <row r="7" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A7" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
-      <c r="K7" s="22"/>
-      <c r="L7" s="22"/>
-      <c r="M7" s="22"/>
-      <c r="N7" s="23"/>
-    </row>
-    <row r="8" spans="1:14" ht="18">
-      <c r="A8" s="42" t="s">
+      <c r="B7" s="19"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="21"/>
+    </row>
+    <row r="8" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A8" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22"/>
-      <c r="J8" s="22"/>
-      <c r="K8" s="22"/>
-      <c r="L8" s="22"/>
-      <c r="M8" s="22"/>
-      <c r="N8" s="23"/>
-    </row>
-    <row r="9" spans="1:14" ht="18">
-      <c r="A9" s="42" t="s">
+      <c r="B8" s="19"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="21"/>
+    </row>
+    <row r="9" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A9" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
-      <c r="J9" s="22"/>
-      <c r="K9" s="22"/>
-      <c r="L9" s="22"/>
-      <c r="M9" s="22"/>
-      <c r="N9" s="23"/>
-    </row>
-    <row r="10" spans="1:14" ht="18">
-      <c r="A10" s="42" t="s">
+      <c r="B9" s="19"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="20"/>
+      <c r="N9" s="21"/>
+    </row>
+    <row r="10" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A10" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="22"/>
-      <c r="J10" s="22"/>
-      <c r="K10" s="22"/>
-      <c r="L10" s="22"/>
-      <c r="M10" s="22"/>
-      <c r="N10" s="23"/>
-    </row>
-    <row r="11" spans="1:14" ht="18.75" thickBot="1">
-      <c r="A11" s="43"/>
-      <c r="B11" s="25"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="26"/>
-      <c r="J11" s="26"/>
-      <c r="K11" s="26"/>
-      <c r="L11" s="26"/>
-      <c r="M11" s="26"/>
-      <c r="N11" s="27"/>
-    </row>
-    <row r="12" spans="1:14" s="1" customFormat="1" ht="18.75" thickBot="1">
-      <c r="A12" s="44" t="s">
+      <c r="B10" s="19"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="21"/>
+    </row>
+    <row r="11" spans="1:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="41"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="24"/>
+      <c r="M11" s="24"/>
+      <c r="N11" s="25"/>
+    </row>
+    <row r="12" spans="1:14" s="1" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="29"/>
-      <c r="C12" s="30"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="30"/>
-      <c r="H12" s="30"/>
-      <c r="I12" s="30"/>
-      <c r="J12" s="30"/>
-      <c r="K12" s="30"/>
-      <c r="L12" s="30"/>
-      <c r="M12" s="30"/>
-      <c r="N12" s="31"/>
-    </row>
-    <row r="13" spans="1:14" ht="18">
-      <c r="A13" s="41" t="s">
+      <c r="B12" s="27"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="28"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="28"/>
+      <c r="M12" s="28"/>
+      <c r="N12" s="29"/>
+    </row>
+    <row r="13" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A13" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="32"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="33"/>
-      <c r="J13" s="33"/>
-      <c r="K13" s="33"/>
-      <c r="L13" s="33"/>
-      <c r="M13" s="33"/>
-      <c r="N13" s="34"/>
-    </row>
-    <row r="14" spans="1:14" ht="18">
-      <c r="A14" s="42" t="s">
+      <c r="B13" s="30"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="31"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="31"/>
+      <c r="J13" s="31"/>
+      <c r="K13" s="31"/>
+      <c r="L13" s="31"/>
+      <c r="M13" s="31"/>
+      <c r="N13" s="32"/>
+    </row>
+    <row r="14" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A14" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="21"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="22"/>
-      <c r="J14" s="22"/>
-      <c r="K14" s="22"/>
-      <c r="L14" s="22"/>
-      <c r="M14" s="22"/>
-      <c r="N14" s="22"/>
-    </row>
-    <row r="15" spans="1:14" ht="18.75" thickBot="1">
-      <c r="A15" s="43"/>
-      <c r="B15" s="25"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="26"/>
-      <c r="K15" s="26"/>
-      <c r="L15" s="26"/>
-      <c r="M15" s="26"/>
-      <c r="N15" s="27"/>
-    </row>
-    <row r="16" spans="1:14" s="1" customFormat="1" ht="18.75" thickBot="1">
-      <c r="A16" s="44" t="s">
+      <c r="B14" s="19"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="20"/>
+      <c r="L14" s="20"/>
+      <c r="M14" s="20"/>
+      <c r="N14" s="20"/>
+    </row>
+    <row r="15" spans="1:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="41"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="24"/>
+      <c r="K15" s="24"/>
+      <c r="L15" s="24"/>
+      <c r="M15" s="24"/>
+      <c r="N15" s="25"/>
+    </row>
+    <row r="16" spans="1:14" s="1" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="29"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="30"/>
-      <c r="H16" s="30"/>
-      <c r="I16" s="30"/>
-      <c r="J16" s="30"/>
-      <c r="K16" s="30"/>
-      <c r="L16" s="30"/>
-      <c r="M16" s="30"/>
-      <c r="N16" s="31"/>
-    </row>
-    <row r="17" spans="1:6" ht="13.5" thickBot="1"/>
-    <row r="18" spans="1:6" ht="18.75" thickBot="1">
-      <c r="A18" s="71" t="s">
+      <c r="B16" s="27"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="28"/>
+      <c r="J16" s="28"/>
+      <c r="K16" s="28"/>
+      <c r="L16" s="28"/>
+      <c r="M16" s="28"/>
+      <c r="N16" s="29"/>
+    </row>
+    <row r="17" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="69" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="72" t="e">
+      <c r="B18" s="70" t="e">
         <f>IRR(B16:N16)</f>
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.75">
+    <row r="19" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="F19" s="3"/>
     </row>
-    <row r="20" spans="1:6" ht="15.75">
+    <row r="20" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="1:6" ht="15.75">
+    <row r="21" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
       <c r="F21" s="3"/>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
     </row>
   </sheetData>

</xml_diff>